<commit_message>
Testing doc & front end demo
</commit_message>
<xml_diff>
--- a/BusinessDocuments/_W11_Project Plan (1).xlsx
+++ b/BusinessDocuments/_W11_Project Plan (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive Data\Computer Science Project\BundleBid\BusinessDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB52334E-E2FB-4DAE-B029-29DEB237501C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A239FF9-DE43-4003-8825-E5EDCC4BAEB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="84">
   <si>
     <t>Color Coding</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>Swetha Bitla, Weili Zhong</t>
+  </si>
+  <si>
+    <t>Test Scripts and Cases</t>
   </si>
 </sst>
 </file>
@@ -1663,6 +1666,124 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1687,156 +1808,59 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="20" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="20" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1868,16 +1892,7 @@
     <xf numFmtId="49" fontId="1" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1886,41 +1901,23 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="20" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="20" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="25" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1928,26 +1925,32 @@
     <xf numFmtId="0" fontId="16" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2322,7 +2325,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="197" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -2333,23 +2336,23 @@
       <c r="E1" s="4"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="157" t="s">
+      <c r="H1" s="199" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="158"/>
-      <c r="J1" s="158"/>
-      <c r="K1" s="158"/>
-      <c r="L1" s="158"/>
-      <c r="M1" s="158"/>
-      <c r="N1" s="158"/>
-      <c r="O1" s="158"/>
-      <c r="P1" s="158"/>
-      <c r="Q1" s="158"/>
-      <c r="R1" s="158"/>
-      <c r="S1" s="158"/>
-      <c r="T1" s="158"/>
-      <c r="U1" s="158"/>
-      <c r="V1" s="159"/>
+      <c r="I1" s="200"/>
+      <c r="J1" s="200"/>
+      <c r="K1" s="200"/>
+      <c r="L1" s="200"/>
+      <c r="M1" s="200"/>
+      <c r="N1" s="200"/>
+      <c r="O1" s="200"/>
+      <c r="P1" s="200"/>
+      <c r="Q1" s="200"/>
+      <c r="R1" s="200"/>
+      <c r="S1" s="200"/>
+      <c r="T1" s="200"/>
+      <c r="U1" s="200"/>
+      <c r="V1" s="201"/>
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="6"/>
@@ -2360,7 +2363,7 @@
       <c r="AD1" s="6"/>
     </row>
     <row r="2" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="156"/>
+      <c r="A2" s="198"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="9" t="s">
@@ -2377,13 +2380,13 @@
       <c r="M2" s="57"/>
       <c r="N2" s="57"/>
       <c r="O2" s="58"/>
-      <c r="P2" s="160"/>
-      <c r="Q2" s="160"/>
-      <c r="R2" s="160"/>
-      <c r="S2" s="160"/>
-      <c r="T2" s="161"/>
-      <c r="U2" s="161"/>
-      <c r="V2" s="162"/>
+      <c r="P2" s="202"/>
+      <c r="Q2" s="202"/>
+      <c r="R2" s="202"/>
+      <c r="S2" s="202"/>
+      <c r="T2" s="203"/>
+      <c r="U2" s="203"/>
+      <c r="V2" s="204"/>
       <c r="W2" s="10"/>
       <c r="X2" s="10"/>
       <c r="Y2" s="10"/>
@@ -2525,10 +2528,10 @@
       <c r="A5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="163" t="s">
+      <c r="B5" s="205" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="164"/>
+      <c r="C5" s="206"/>
       <c r="D5" s="29" t="s">
         <v>26</v>
       </c>
@@ -2566,13 +2569,13 @@
       <c r="AD5" s="10"/>
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="184" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="179" t="s">
+      <c r="B6" s="187" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="180"/>
       <c r="D6" s="60" t="s">
         <v>20</v>
       </c>
@@ -2610,11 +2613,11 @@
       <c r="AD6" s="10"/>
     </row>
     <row r="7" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="177"/>
-      <c r="B7" s="180" t="s">
+      <c r="A7" s="193"/>
+      <c r="B7" s="195" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="181"/>
+      <c r="C7" s="196"/>
       <c r="D7" s="60" t="s">
         <v>20</v>
       </c>
@@ -2652,11 +2655,11 @@
       <c r="AD7" s="59"/>
     </row>
     <row r="8" spans="1:30" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="177"/>
-      <c r="B8" s="179" t="s">
+      <c r="A8" s="193"/>
+      <c r="B8" s="187" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="180"/>
       <c r="D8" s="60" t="s">
         <v>63</v>
       </c>
@@ -2694,11 +2697,11 @@
       <c r="AD8" s="10"/>
     </row>
     <row r="9" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="177"/>
-      <c r="B9" s="179" t="s">
+      <c r="A9" s="193"/>
+      <c r="B9" s="187" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="173"/>
+      <c r="C9" s="180"/>
       <c r="D9" s="60" t="s">
         <v>55</v>
       </c>
@@ -2736,11 +2739,11 @@
       <c r="AD9" s="10"/>
     </row>
     <row r="10" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="178"/>
-      <c r="B10" s="165" t="s">
+      <c r="A10" s="194"/>
+      <c r="B10" s="188" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="166"/>
+      <c r="C10" s="189"/>
       <c r="D10" s="60" t="s">
         <v>55</v>
       </c>
@@ -2778,30 +2781,30 @@
       <c r="AD10" s="59"/>
     </row>
     <row r="11" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="167" t="s">
+      <c r="A11" s="190" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="168"/>
-      <c r="C11" s="168"/>
-      <c r="D11" s="168"/>
-      <c r="E11" s="168"/>
-      <c r="F11" s="168"/>
-      <c r="G11" s="168"/>
-      <c r="H11" s="168"/>
-      <c r="I11" s="168"/>
-      <c r="J11" s="168"/>
-      <c r="K11" s="168"/>
-      <c r="L11" s="168"/>
-      <c r="M11" s="168"/>
-      <c r="N11" s="168"/>
-      <c r="O11" s="168"/>
-      <c r="P11" s="168"/>
-      <c r="Q11" s="168"/>
-      <c r="R11" s="168"/>
-      <c r="S11" s="168"/>
-      <c r="T11" s="168"/>
-      <c r="U11" s="168"/>
-      <c r="V11" s="169"/>
+      <c r="B11" s="182"/>
+      <c r="C11" s="182"/>
+      <c r="D11" s="182"/>
+      <c r="E11" s="182"/>
+      <c r="F11" s="182"/>
+      <c r="G11" s="182"/>
+      <c r="H11" s="182"/>
+      <c r="I11" s="182"/>
+      <c r="J11" s="182"/>
+      <c r="K11" s="182"/>
+      <c r="L11" s="182"/>
+      <c r="M11" s="182"/>
+      <c r="N11" s="182"/>
+      <c r="O11" s="182"/>
+      <c r="P11" s="182"/>
+      <c r="Q11" s="182"/>
+      <c r="R11" s="182"/>
+      <c r="S11" s="182"/>
+      <c r="T11" s="182"/>
+      <c r="U11" s="182"/>
+      <c r="V11" s="183"/>
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
@@ -2812,13 +2815,13 @@
       <c r="AD11" s="10"/>
     </row>
     <row r="12" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="170" t="s">
+      <c r="A12" s="191" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="172" t="s">
+      <c r="B12" s="179" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="173"/>
+      <c r="C12" s="180"/>
       <c r="D12" s="60" t="s">
         <v>53</v>
       </c>
@@ -2856,11 +2859,11 @@
       <c r="AD12" s="10"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="170"/>
-      <c r="B13" s="172" t="s">
+      <c r="A13" s="191"/>
+      <c r="B13" s="179" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="173"/>
+      <c r="C13" s="180"/>
       <c r="D13" s="60" t="s">
         <v>56</v>
       </c>
@@ -2898,11 +2901,11 @@
       <c r="AD13" s="10"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="170"/>
-      <c r="B14" s="172" t="s">
+      <c r="A14" s="191"/>
+      <c r="B14" s="179" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="173"/>
+      <c r="C14" s="180"/>
       <c r="D14" s="60" t="s">
         <v>52</v>
       </c>
@@ -2940,11 +2943,11 @@
       <c r="AD14" s="10"/>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="170"/>
-      <c r="B15" s="172" t="s">
+      <c r="A15" s="191"/>
+      <c r="B15" s="179" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="173"/>
+      <c r="C15" s="180"/>
       <c r="D15" s="72" t="s">
         <v>41</v>
       </c>
@@ -2982,11 +2985,11 @@
       <c r="AD15" s="10"/>
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="170"/>
-      <c r="B16" s="174" t="s">
+      <c r="A16" s="191"/>
+      <c r="B16" s="178" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="175"/>
+      <c r="C16" s="167"/>
       <c r="D16" s="72" t="s">
         <v>41</v>
       </c>
@@ -3024,11 +3027,11 @@
       <c r="AD16" s="59"/>
     </row>
     <row r="17" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="170"/>
-      <c r="B17" s="174" t="s">
+      <c r="A17" s="191"/>
+      <c r="B17" s="178" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="175"/>
+      <c r="C17" s="167"/>
       <c r="D17" s="60" t="s">
         <v>52</v>
       </c>
@@ -3066,11 +3069,11 @@
       <c r="AD17" s="59"/>
     </row>
     <row r="18" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="170"/>
-      <c r="B18" s="174" t="s">
+      <c r="A18" s="191"/>
+      <c r="B18" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="175"/>
+      <c r="C18" s="167"/>
       <c r="D18" s="72" t="s">
         <v>41</v>
       </c>
@@ -3108,11 +3111,11 @@
       <c r="AD18" s="59"/>
     </row>
     <row r="19" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="170"/>
-      <c r="B19" s="174" t="s">
+      <c r="A19" s="191"/>
+      <c r="B19" s="178" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="175"/>
+      <c r="C19" s="167"/>
       <c r="D19" s="60" t="s">
         <v>52</v>
       </c>
@@ -3150,11 +3153,11 @@
       <c r="AD19" s="59"/>
     </row>
     <row r="20" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="170"/>
-      <c r="B20" s="174" t="s">
+      <c r="A20" s="191"/>
+      <c r="B20" s="178" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="175"/>
+      <c r="C20" s="167"/>
       <c r="D20" s="60" t="s">
         <v>52</v>
       </c>
@@ -3192,11 +3195,11 @@
       <c r="AD20" s="59"/>
     </row>
     <row r="21" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="171"/>
-      <c r="B21" s="172" t="s">
+      <c r="A21" s="192"/>
+      <c r="B21" s="179" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="173"/>
+      <c r="C21" s="180"/>
       <c r="D21" s="72" t="s">
         <v>55</v>
       </c>
@@ -3234,30 +3237,30 @@
       <c r="AD21" s="10"/>
     </row>
     <row r="22" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="187" t="s">
+      <c r="A22" s="181" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="168"/>
-      <c r="C22" s="168"/>
-      <c r="D22" s="168"/>
-      <c r="E22" s="168"/>
-      <c r="F22" s="168"/>
-      <c r="G22" s="168"/>
-      <c r="H22" s="168"/>
-      <c r="I22" s="168"/>
-      <c r="J22" s="168"/>
-      <c r="K22" s="168"/>
-      <c r="L22" s="168"/>
-      <c r="M22" s="168"/>
-      <c r="N22" s="168"/>
-      <c r="O22" s="168"/>
-      <c r="P22" s="168"/>
-      <c r="Q22" s="168"/>
-      <c r="R22" s="168"/>
-      <c r="S22" s="168"/>
-      <c r="T22" s="168"/>
-      <c r="U22" s="168"/>
-      <c r="V22" s="169"/>
+      <c r="B22" s="182"/>
+      <c r="C22" s="182"/>
+      <c r="D22" s="182"/>
+      <c r="E22" s="182"/>
+      <c r="F22" s="182"/>
+      <c r="G22" s="182"/>
+      <c r="H22" s="182"/>
+      <c r="I22" s="182"/>
+      <c r="J22" s="182"/>
+      <c r="K22" s="182"/>
+      <c r="L22" s="182"/>
+      <c r="M22" s="182"/>
+      <c r="N22" s="182"/>
+      <c r="O22" s="182"/>
+      <c r="P22" s="182"/>
+      <c r="Q22" s="182"/>
+      <c r="R22" s="182"/>
+      <c r="S22" s="182"/>
+      <c r="T22" s="182"/>
+      <c r="U22" s="182"/>
+      <c r="V22" s="183"/>
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
@@ -3268,13 +3271,13 @@
       <c r="AD22" s="10"/>
     </row>
     <row r="23" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="176" t="s">
+      <c r="A23" s="184" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="172" t="s">
+      <c r="B23" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="173"/>
+      <c r="C23" s="180"/>
       <c r="D23" s="60" t="s">
         <v>64</v>
       </c>
@@ -3312,11 +3315,11 @@
       <c r="AD23" s="10"/>
     </row>
     <row r="24" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="188"/>
-      <c r="B24" s="172" t="s">
+      <c r="A24" s="185"/>
+      <c r="B24" s="179" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="173"/>
+      <c r="C24" s="180"/>
       <c r="D24" s="60" t="s">
         <v>56</v>
       </c>
@@ -3354,11 +3357,11 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="188"/>
-      <c r="B25" s="179" t="s">
+      <c r="A25" s="185"/>
+      <c r="B25" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="173"/>
+      <c r="C25" s="180"/>
       <c r="D25" s="60" t="s">
         <v>64</v>
       </c>
@@ -3396,11 +3399,11 @@
       <c r="AD25" s="10"/>
     </row>
     <row r="26" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="189"/>
-      <c r="B26" s="179" t="s">
+      <c r="A26" s="186"/>
+      <c r="B26" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="173"/>
+      <c r="C26" s="180"/>
       <c r="D26" s="60" t="s">
         <v>52</v>
       </c>
@@ -3438,30 +3441,30 @@
       <c r="AD26" s="10"/>
     </row>
     <row r="27" spans="1:30" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="182" t="s">
+      <c r="A27" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="183"/>
-      <c r="C27" s="183"/>
-      <c r="D27" s="183"/>
-      <c r="E27" s="183"/>
-      <c r="F27" s="183"/>
-      <c r="G27" s="183"/>
-      <c r="H27" s="183"/>
-      <c r="I27" s="183"/>
-      <c r="J27" s="183"/>
-      <c r="K27" s="183"/>
-      <c r="L27" s="183"/>
-      <c r="M27" s="183"/>
-      <c r="N27" s="183"/>
-      <c r="O27" s="183"/>
-      <c r="P27" s="183"/>
-      <c r="Q27" s="183"/>
-      <c r="R27" s="183"/>
-      <c r="S27" s="183"/>
-      <c r="T27" s="183"/>
-      <c r="U27" s="183"/>
-      <c r="V27" s="184"/>
+      <c r="B27" s="174"/>
+      <c r="C27" s="174"/>
+      <c r="D27" s="174"/>
+      <c r="E27" s="174"/>
+      <c r="F27" s="174"/>
+      <c r="G27" s="174"/>
+      <c r="H27" s="174"/>
+      <c r="I27" s="174"/>
+      <c r="J27" s="174"/>
+      <c r="K27" s="174"/>
+      <c r="L27" s="174"/>
+      <c r="M27" s="174"/>
+      <c r="N27" s="174"/>
+      <c r="O27" s="174"/>
+      <c r="P27" s="174"/>
+      <c r="Q27" s="174"/>
+      <c r="R27" s="174"/>
+      <c r="S27" s="174"/>
+      <c r="T27" s="174"/>
+      <c r="U27" s="174"/>
+      <c r="V27" s="175"/>
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
@@ -3472,13 +3475,13 @@
       <c r="AD27" s="10"/>
     </row>
     <row r="28" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="185" t="s">
+      <c r="A28" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="194" t="s">
+      <c r="B28" s="164" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="195"/>
+      <c r="C28" s="165"/>
       <c r="D28" s="60" t="s">
         <v>64</v>
       </c>
@@ -3516,11 +3519,11 @@
       <c r="AD28" s="10"/>
     </row>
     <row r="29" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="186"/>
-      <c r="B29" s="196" t="s">
+      <c r="A29" s="177"/>
+      <c r="B29" s="166" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="175"/>
+      <c r="C29" s="167"/>
       <c r="D29" s="60" t="s">
         <v>64</v>
       </c>
@@ -3558,30 +3561,30 @@
       <c r="AD29" s="10"/>
     </row>
     <row r="30" spans="1:30" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="197" t="s">
+      <c r="A30" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="198"/>
-      <c r="C30" s="198"/>
-      <c r="D30" s="198"/>
-      <c r="E30" s="198"/>
-      <c r="F30" s="198"/>
-      <c r="G30" s="198"/>
-      <c r="H30" s="198"/>
-      <c r="I30" s="198"/>
-      <c r="J30" s="198"/>
-      <c r="K30" s="198"/>
-      <c r="L30" s="198"/>
-      <c r="M30" s="198"/>
-      <c r="N30" s="198"/>
-      <c r="O30" s="198"/>
-      <c r="P30" s="198"/>
-      <c r="Q30" s="198"/>
-      <c r="R30" s="198"/>
-      <c r="S30" s="198"/>
-      <c r="T30" s="198"/>
-      <c r="U30" s="198"/>
-      <c r="V30" s="199"/>
+      <c r="B30" s="169"/>
+      <c r="C30" s="169"/>
+      <c r="D30" s="169"/>
+      <c r="E30" s="169"/>
+      <c r="F30" s="169"/>
+      <c r="G30" s="169"/>
+      <c r="H30" s="169"/>
+      <c r="I30" s="169"/>
+      <c r="J30" s="169"/>
+      <c r="K30" s="169"/>
+      <c r="L30" s="169"/>
+      <c r="M30" s="169"/>
+      <c r="N30" s="169"/>
+      <c r="O30" s="169"/>
+      <c r="P30" s="169"/>
+      <c r="Q30" s="169"/>
+      <c r="R30" s="169"/>
+      <c r="S30" s="169"/>
+      <c r="T30" s="169"/>
+      <c r="U30" s="169"/>
+      <c r="V30" s="170"/>
       <c r="W30" s="10"/>
       <c r="X30" s="10"/>
       <c r="Y30" s="10"/>
@@ -3592,13 +3595,13 @@
       <c r="AD30" s="10"/>
     </row>
     <row r="31" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="200" t="s">
+      <c r="A31" s="171" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="196" t="s">
+      <c r="B31" s="166" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="175"/>
+      <c r="C31" s="167"/>
       <c r="D31" s="74" t="s">
         <v>54</v>
       </c>
@@ -3636,11 +3639,11 @@
       <c r="AD31" s="10"/>
     </row>
     <row r="32" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="201"/>
-      <c r="B32" s="196" t="s">
+      <c r="A32" s="172"/>
+      <c r="B32" s="166" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="175"/>
+      <c r="C32" s="167"/>
       <c r="D32" s="74" t="s">
         <v>54</v>
       </c>
@@ -3678,11 +3681,11 @@
       <c r="AD32" s="10"/>
     </row>
     <row r="33" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="201"/>
-      <c r="B33" s="196" t="s">
+      <c r="A33" s="172"/>
+      <c r="B33" s="166" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="175"/>
+      <c r="C33" s="167"/>
       <c r="D33" s="74" t="s">
         <v>54</v>
       </c>
@@ -3720,11 +3723,11 @@
       <c r="AD33" s="10"/>
     </row>
     <row r="34" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="201"/>
-      <c r="B34" s="196" t="s">
+      <c r="A34" s="172"/>
+      <c r="B34" s="166" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="175"/>
+      <c r="C34" s="167"/>
       <c r="D34" s="74" t="s">
         <v>54</v>
       </c>
@@ -3762,11 +3765,11 @@
       <c r="AD34" s="10"/>
     </row>
     <row r="35" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="201"/>
-      <c r="B35" s="196" t="s">
+      <c r="A35" s="172"/>
+      <c r="B35" s="166" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="175"/>
+      <c r="C35" s="167"/>
       <c r="D35" s="72" t="s">
         <v>20</v>
       </c>
@@ -3804,30 +3807,30 @@
       <c r="AD35" s="10"/>
     </row>
     <row r="36" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="190" t="s">
+      <c r="A36" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="190"/>
-      <c r="C36" s="190"/>
-      <c r="D36" s="190"/>
-      <c r="E36" s="190"/>
-      <c r="F36" s="190"/>
-      <c r="G36" s="190"/>
-      <c r="H36" s="190"/>
-      <c r="I36" s="190"/>
-      <c r="J36" s="190"/>
-      <c r="K36" s="190"/>
-      <c r="L36" s="190"/>
-      <c r="M36" s="190"/>
-      <c r="N36" s="190"/>
-      <c r="O36" s="190"/>
-      <c r="P36" s="190"/>
-      <c r="Q36" s="190"/>
-      <c r="R36" s="190"/>
-      <c r="S36" s="190"/>
-      <c r="T36" s="190"/>
-      <c r="U36" s="190"/>
-      <c r="V36" s="191"/>
+      <c r="B36" s="160"/>
+      <c r="C36" s="160"/>
+      <c r="D36" s="160"/>
+      <c r="E36" s="160"/>
+      <c r="F36" s="160"/>
+      <c r="G36" s="160"/>
+      <c r="H36" s="160"/>
+      <c r="I36" s="160"/>
+      <c r="J36" s="160"/>
+      <c r="K36" s="160"/>
+      <c r="L36" s="160"/>
+      <c r="M36" s="160"/>
+      <c r="N36" s="160"/>
+      <c r="O36" s="160"/>
+      <c r="P36" s="160"/>
+      <c r="Q36" s="160"/>
+      <c r="R36" s="160"/>
+      <c r="S36" s="160"/>
+      <c r="T36" s="160"/>
+      <c r="U36" s="160"/>
+      <c r="V36" s="161"/>
       <c r="W36" s="10"/>
       <c r="X36" s="10"/>
       <c r="Y36" s="10"/>
@@ -3841,10 +3844,10 @@
       <c r="A37" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="192" t="s">
+      <c r="B37" s="162" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="193"/>
+      <c r="C37" s="163"/>
       <c r="D37" s="74" t="s">
         <v>20</v>
       </c>
@@ -32875,28 +32878,11 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A36:V36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A30:V30"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A27:V27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A22:V22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H1:V1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="A11:V11"/>
     <mergeCell ref="A12:A21"/>
@@ -32912,11 +32898,28 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:V1"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A27:V27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A22:V22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A36:V36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A30:V30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -32927,8 +32930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -32947,7 +32950,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="197" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="130"/>
@@ -32958,23 +32961,23 @@
       <c r="E1" s="4"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="157" t="s">
+      <c r="H1" s="199" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="158"/>
-      <c r="J1" s="158"/>
-      <c r="K1" s="158"/>
-      <c r="L1" s="158"/>
-      <c r="M1" s="158"/>
-      <c r="N1" s="158"/>
-      <c r="O1" s="158"/>
-      <c r="P1" s="158"/>
-      <c r="Q1" s="158"/>
-      <c r="R1" s="158"/>
-      <c r="S1" s="158"/>
-      <c r="T1" s="158"/>
-      <c r="U1" s="158"/>
-      <c r="V1" s="159"/>
+      <c r="I1" s="200"/>
+      <c r="J1" s="200"/>
+      <c r="K1" s="200"/>
+      <c r="L1" s="200"/>
+      <c r="M1" s="200"/>
+      <c r="N1" s="200"/>
+      <c r="O1" s="200"/>
+      <c r="P1" s="200"/>
+      <c r="Q1" s="200"/>
+      <c r="R1" s="200"/>
+      <c r="S1" s="200"/>
+      <c r="T1" s="200"/>
+      <c r="U1" s="200"/>
+      <c r="V1" s="201"/>
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="6"/>
@@ -32985,7 +32988,7 @@
       <c r="AD1" s="6"/>
     </row>
     <row r="2" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="156"/>
+      <c r="A2" s="198"/>
       <c r="B2" s="131"/>
       <c r="C2" s="132"/>
       <c r="D2" s="9" t="s">
@@ -33002,13 +33005,13 @@
       <c r="M2" s="57"/>
       <c r="N2" s="57"/>
       <c r="O2" s="58"/>
-      <c r="P2" s="160"/>
-      <c r="Q2" s="160"/>
-      <c r="R2" s="160"/>
-      <c r="S2" s="160"/>
-      <c r="T2" s="161"/>
-      <c r="U2" s="161"/>
-      <c r="V2" s="162"/>
+      <c r="P2" s="202"/>
+      <c r="Q2" s="202"/>
+      <c r="R2" s="202"/>
+      <c r="S2" s="202"/>
+      <c r="T2" s="203"/>
+      <c r="U2" s="203"/>
+      <c r="V2" s="204"/>
       <c r="W2" s="10"/>
       <c r="X2" s="10"/>
       <c r="Y2" s="10"/>
@@ -33150,10 +33153,10 @@
       <c r="A5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="232" t="s">
+      <c r="B5" s="236" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="233"/>
+      <c r="C5" s="237"/>
       <c r="D5" s="29" t="s">
         <v>26</v>
       </c>
@@ -33191,13 +33194,13 @@
       <c r="AD5" s="10"/>
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="225" t="s">
+      <c r="A6" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="209" t="s">
+      <c r="B6" s="238" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="210"/>
+      <c r="C6" s="239"/>
       <c r="D6" s="85" t="s">
         <v>20</v>
       </c>
@@ -33235,11 +33238,11 @@
       <c r="AD6" s="10"/>
     </row>
     <row r="7" spans="1:30" s="56" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="226"/>
-      <c r="B7" s="207" t="s">
+      <c r="A7" s="233"/>
+      <c r="B7" s="240" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="208"/>
+      <c r="C7" s="241"/>
       <c r="D7" s="85" t="s">
         <v>20</v>
       </c>
@@ -33277,12 +33280,12 @@
       <c r="AD7" s="59"/>
     </row>
     <row r="8" spans="1:30" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="226"/>
-      <c r="B8" s="209" t="s">
+      <c r="A8" s="233"/>
+      <c r="B8" s="238" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="210"/>
-      <c r="D8" s="242" t="s">
+      <c r="C8" s="239"/>
+      <c r="D8" s="155" t="s">
         <v>63</v>
       </c>
       <c r="E8" s="84">
@@ -33319,11 +33322,11 @@
       <c r="AD8" s="10"/>
     </row>
     <row r="9" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="226"/>
-      <c r="B9" s="209" t="s">
+      <c r="A9" s="233"/>
+      <c r="B9" s="238" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="210"/>
+      <c r="C9" s="239"/>
       <c r="D9" s="85" t="s">
         <v>55</v>
       </c>
@@ -33361,11 +33364,11 @@
       <c r="AD9" s="10"/>
     </row>
     <row r="10" spans="1:30" s="56" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="227"/>
-      <c r="B10" s="211" t="s">
+      <c r="A10" s="234"/>
+      <c r="B10" s="242" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="212"/>
+      <c r="C10" s="243"/>
       <c r="D10" s="85" t="s">
         <v>55</v>
       </c>
@@ -33403,30 +33406,30 @@
       <c r="AD10" s="59"/>
     </row>
     <row r="11" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="167" t="s">
+      <c r="A11" s="190" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="168"/>
-      <c r="C11" s="224"/>
-      <c r="D11" s="168"/>
-      <c r="E11" s="168"/>
-      <c r="F11" s="168"/>
-      <c r="G11" s="168"/>
-      <c r="H11" s="168"/>
-      <c r="I11" s="168"/>
-      <c r="J11" s="168"/>
-      <c r="K11" s="168"/>
-      <c r="L11" s="168"/>
-      <c r="M11" s="168"/>
-      <c r="N11" s="168"/>
-      <c r="O11" s="168"/>
-      <c r="P11" s="168"/>
-      <c r="Q11" s="168"/>
-      <c r="R11" s="168"/>
-      <c r="S11" s="168"/>
-      <c r="T11" s="168"/>
-      <c r="U11" s="168"/>
-      <c r="V11" s="169"/>
+      <c r="B11" s="182"/>
+      <c r="C11" s="231"/>
+      <c r="D11" s="182"/>
+      <c r="E11" s="182"/>
+      <c r="F11" s="182"/>
+      <c r="G11" s="182"/>
+      <c r="H11" s="182"/>
+      <c r="I11" s="182"/>
+      <c r="J11" s="182"/>
+      <c r="K11" s="182"/>
+      <c r="L11" s="182"/>
+      <c r="M11" s="182"/>
+      <c r="N11" s="182"/>
+      <c r="O11" s="182"/>
+      <c r="P11" s="182"/>
+      <c r="Q11" s="182"/>
+      <c r="R11" s="182"/>
+      <c r="S11" s="182"/>
+      <c r="T11" s="182"/>
+      <c r="U11" s="182"/>
+      <c r="V11" s="183"/>
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
@@ -33437,13 +33440,13 @@
       <c r="AD11" s="10"/>
     </row>
     <row r="12" spans="1:30" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="222" t="s">
+      <c r="A12" s="229" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="228" t="s">
+      <c r="B12" s="210" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="229"/>
+      <c r="C12" s="211"/>
       <c r="D12" s="133" t="s">
         <v>56</v>
       </c>
@@ -33481,11 +33484,11 @@
       <c r="AD12" s="10"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="222"/>
-      <c r="B13" s="228" t="s">
+      <c r="A13" s="229"/>
+      <c r="B13" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="229"/>
+      <c r="C13" s="211"/>
       <c r="D13" s="134" t="s">
         <v>52</v>
       </c>
@@ -33523,7 +33526,7 @@
       <c r="AD13" s="10"/>
     </row>
     <row r="14" spans="1:30" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="222"/>
+      <c r="A14" s="229"/>
       <c r="B14" s="136" t="s">
         <v>65</v>
       </c>
@@ -33565,7 +33568,7 @@
       <c r="AD14" s="59"/>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="222"/>
+      <c r="A15" s="229"/>
       <c r="B15" s="137" t="s">
         <v>38</v>
       </c>
@@ -33607,11 +33610,11 @@
       <c r="AD15" s="10"/>
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="222"/>
-      <c r="B16" s="228" t="s">
+      <c r="A16" s="229"/>
+      <c r="B16" s="210" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="229"/>
+      <c r="C16" s="211"/>
       <c r="D16" s="142" t="s">
         <v>52</v>
       </c>
@@ -33649,11 +33652,11 @@
       <c r="AD16" s="10"/>
     </row>
     <row r="17" spans="1:30" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="222"/>
-      <c r="B17" s="228" t="s">
+      <c r="A17" s="229"/>
+      <c r="B17" s="210" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="229"/>
+      <c r="C17" s="211"/>
       <c r="D17" s="35" t="s">
         <v>55</v>
       </c>
@@ -33691,11 +33694,11 @@
       <c r="AD17" s="59"/>
     </row>
     <row r="18" spans="1:30" s="56" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="222"/>
-      <c r="B18" s="237" t="s">
+      <c r="A18" s="229"/>
+      <c r="B18" s="212" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="231"/>
+      <c r="C18" s="213"/>
       <c r="D18" s="144" t="s">
         <v>67</v>
       </c>
@@ -33733,11 +33736,11 @@
       <c r="AD18" s="59"/>
     </row>
     <row r="19" spans="1:30" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="222"/>
-      <c r="B19" s="228" t="s">
+      <c r="A19" s="229"/>
+      <c r="B19" s="210" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="229"/>
+      <c r="C19" s="211"/>
       <c r="D19" s="35" t="s">
         <v>41</v>
       </c>
@@ -33775,11 +33778,11 @@
       <c r="AD19" s="59"/>
     </row>
     <row r="20" spans="1:30" s="56" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="222"/>
-      <c r="B20" s="230" t="s">
+      <c r="A20" s="229"/>
+      <c r="B20" s="235" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="231"/>
+      <c r="C20" s="213"/>
       <c r="D20" s="154" t="s">
         <v>72</v>
       </c>
@@ -33817,11 +33820,11 @@
       <c r="AD20" s="59"/>
     </row>
     <row r="21" spans="1:30" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="222"/>
-      <c r="B21" s="228" t="s">
+      <c r="A21" s="229"/>
+      <c r="B21" s="210" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="229"/>
+      <c r="C21" s="211"/>
       <c r="D21" s="134" t="s">
         <v>64</v>
       </c>
@@ -33859,11 +33862,11 @@
       <c r="AD21" s="59"/>
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="223"/>
-      <c r="B22" s="228" t="s">
+      <c r="A22" s="230"/>
+      <c r="B22" s="210" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="229"/>
+      <c r="C22" s="211"/>
       <c r="D22" s="35" t="s">
         <v>55</v>
       </c>
@@ -33901,30 +33904,30 @@
       <c r="AD22" s="10"/>
     </row>
     <row r="23" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="187" t="s">
+      <c r="A23" s="181" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="168"/>
-      <c r="C23" s="224"/>
-      <c r="D23" s="168"/>
-      <c r="E23" s="168"/>
-      <c r="F23" s="168"/>
-      <c r="G23" s="168"/>
-      <c r="H23" s="168"/>
-      <c r="I23" s="168"/>
-      <c r="J23" s="168"/>
-      <c r="K23" s="168"/>
-      <c r="L23" s="168"/>
-      <c r="M23" s="168"/>
-      <c r="N23" s="168"/>
-      <c r="O23" s="168"/>
-      <c r="P23" s="168"/>
-      <c r="Q23" s="168"/>
-      <c r="R23" s="168"/>
-      <c r="S23" s="168"/>
-      <c r="T23" s="168"/>
-      <c r="U23" s="168"/>
-      <c r="V23" s="169"/>
+      <c r="B23" s="182"/>
+      <c r="C23" s="231"/>
+      <c r="D23" s="182"/>
+      <c r="E23" s="182"/>
+      <c r="F23" s="182"/>
+      <c r="G23" s="182"/>
+      <c r="H23" s="182"/>
+      <c r="I23" s="182"/>
+      <c r="J23" s="182"/>
+      <c r="K23" s="182"/>
+      <c r="L23" s="182"/>
+      <c r="M23" s="182"/>
+      <c r="N23" s="182"/>
+      <c r="O23" s="182"/>
+      <c r="P23" s="182"/>
+      <c r="Q23" s="182"/>
+      <c r="R23" s="182"/>
+      <c r="S23" s="182"/>
+      <c r="T23" s="182"/>
+      <c r="U23" s="182"/>
+      <c r="V23" s="183"/>
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
@@ -33935,13 +33938,13 @@
       <c r="AD23" s="10"/>
     </row>
     <row r="24" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="218" t="s">
+      <c r="A24" s="225" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="214" t="s">
+      <c r="B24" s="246" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="215"/>
+      <c r="C24" s="247"/>
       <c r="D24" s="152" t="s">
         <v>53</v>
       </c>
@@ -33979,7 +33982,7 @@
       <c r="AD24" s="10"/>
     </row>
     <row r="25" spans="1:30" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="219"/>
+      <c r="A25" s="226"/>
       <c r="B25" s="149" t="s">
         <v>71</v>
       </c>
@@ -34021,11 +34024,11 @@
       <c r="AD25" s="59"/>
     </row>
     <row r="26" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="220"/>
-      <c r="B26" s="214" t="s">
+      <c r="A26" s="227"/>
+      <c r="B26" s="246" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="215"/>
+      <c r="C26" s="247"/>
       <c r="D26" s="152" t="s">
         <v>55</v>
       </c>
@@ -34063,11 +34066,11 @@
       <c r="AD26" s="10"/>
     </row>
     <row r="27" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="220"/>
-      <c r="B27" s="216" t="s">
+      <c r="A27" s="227"/>
+      <c r="B27" s="248" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="217"/>
+      <c r="C27" s="249"/>
       <c r="D27" s="100" t="s">
         <v>56</v>
       </c>
@@ -34105,11 +34108,11 @@
       <c r="AD27" s="10"/>
     </row>
     <row r="28" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="221"/>
-      <c r="B28" s="216" t="s">
+      <c r="A28" s="228"/>
+      <c r="B28" s="248" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="217"/>
+      <c r="C28" s="249"/>
       <c r="D28" s="100" t="s">
         <v>54</v>
       </c>
@@ -34147,30 +34150,30 @@
       <c r="AD28" s="10"/>
     </row>
     <row r="29" spans="1:30" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="182" t="s">
+      <c r="A29" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="183"/>
-      <c r="C29" s="224"/>
-      <c r="D29" s="183"/>
-      <c r="E29" s="183"/>
-      <c r="F29" s="183"/>
-      <c r="G29" s="183"/>
-      <c r="H29" s="183"/>
-      <c r="I29" s="183"/>
-      <c r="J29" s="183"/>
-      <c r="K29" s="183"/>
-      <c r="L29" s="183"/>
-      <c r="M29" s="183"/>
-      <c r="N29" s="183"/>
-      <c r="O29" s="183"/>
-      <c r="P29" s="183"/>
-      <c r="Q29" s="183"/>
-      <c r="R29" s="183"/>
-      <c r="S29" s="183"/>
-      <c r="T29" s="183"/>
-      <c r="U29" s="183"/>
-      <c r="V29" s="184"/>
+      <c r="B29" s="174"/>
+      <c r="C29" s="231"/>
+      <c r="D29" s="174"/>
+      <c r="E29" s="174"/>
+      <c r="F29" s="174"/>
+      <c r="G29" s="174"/>
+      <c r="H29" s="174"/>
+      <c r="I29" s="174"/>
+      <c r="J29" s="174"/>
+      <c r="K29" s="174"/>
+      <c r="L29" s="174"/>
+      <c r="M29" s="174"/>
+      <c r="N29" s="174"/>
+      <c r="O29" s="174"/>
+      <c r="P29" s="174"/>
+      <c r="Q29" s="174"/>
+      <c r="R29" s="174"/>
+      <c r="S29" s="174"/>
+      <c r="T29" s="174"/>
+      <c r="U29" s="174"/>
+      <c r="V29" s="175"/>
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10"/>
@@ -34181,22 +34184,22 @@
       <c r="AD29" s="10"/>
     </row>
     <row r="30" spans="1:30" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="238" t="s">
+      <c r="A30" s="214" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="249" t="s">
+      <c r="B30" s="219" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="151" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="251" t="s">
+      <c r="D30" s="221" t="s">
         <v>79</v>
       </c>
       <c r="E30" s="83">
         <v>43922</v>
       </c>
-      <c r="F30" s="248">
+      <c r="F30" s="158">
         <v>43935</v>
       </c>
       <c r="G30" s="118">
@@ -34227,20 +34230,20 @@
       <c r="AD30" s="10"/>
     </row>
     <row r="31" spans="1:30" s="56" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="238"/>
-      <c r="B31" s="249"/>
-      <c r="C31" s="244" t="s">
+      <c r="A31" s="214"/>
+      <c r="B31" s="219"/>
+      <c r="C31" s="156" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="238"/>
+      <c r="D31" s="214"/>
       <c r="E31" s="83">
         <v>43922</v>
       </c>
-      <c r="F31" s="248">
+      <c r="F31" s="158">
         <v>43935</v>
       </c>
       <c r="G31" s="118">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H31" s="112"/>
       <c r="I31" s="112"/>
@@ -34267,16 +34270,16 @@
       <c r="AD31" s="59"/>
     </row>
     <row r="32" spans="1:30" s="56" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="238"/>
-      <c r="B32" s="249"/>
-      <c r="C32" s="244" t="s">
+      <c r="A32" s="214"/>
+      <c r="B32" s="219"/>
+      <c r="C32" s="156" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="238"/>
+      <c r="D32" s="214"/>
       <c r="E32" s="83">
         <v>43922</v>
       </c>
-      <c r="F32" s="248">
+      <c r="F32" s="158">
         <v>43935</v>
       </c>
       <c r="G32" s="118">
@@ -34307,20 +34310,20 @@
       <c r="AD32" s="59"/>
     </row>
     <row r="33" spans="1:30" s="56" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="243"/>
-      <c r="B33" s="250"/>
-      <c r="C33" s="245" t="s">
+      <c r="A33" s="215"/>
+      <c r="B33" s="220"/>
+      <c r="C33" s="157" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="239"/>
+      <c r="D33" s="222"/>
       <c r="E33" s="83">
         <v>43922</v>
       </c>
-      <c r="F33" s="248">
+      <c r="F33" s="158">
         <v>43935</v>
       </c>
       <c r="G33" s="118">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="H33" s="112"/>
       <c r="I33" s="112"/>
@@ -34347,14 +34350,14 @@
       <c r="AD33" s="59"/>
     </row>
     <row r="34" spans="1:30" s="56" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="238"/>
-      <c r="B34" s="246" t="s">
+      <c r="A34" s="214"/>
+      <c r="B34" s="244" t="s">
         <v>60</v>
       </c>
       <c r="C34" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="252" t="s">
+      <c r="D34" s="223" t="s">
         <v>79</v>
       </c>
       <c r="E34" s="83">
@@ -34391,12 +34394,12 @@
       <c r="AD34" s="59"/>
     </row>
     <row r="35" spans="1:30" s="56" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="238"/>
-      <c r="B35" s="247"/>
+      <c r="A35" s="214"/>
+      <c r="B35" s="245"/>
       <c r="C35" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="213"/>
+      <c r="D35" s="224"/>
       <c r="E35" s="83">
         <v>43922</v>
       </c>
@@ -34431,30 +34434,30 @@
       <c r="AD35" s="59"/>
     </row>
     <row r="36" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="197" t="s">
+      <c r="A36" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="197"/>
-      <c r="C36" s="197"/>
-      <c r="D36" s="197"/>
-      <c r="E36" s="197"/>
-      <c r="F36" s="197"/>
-      <c r="G36" s="197"/>
-      <c r="H36" s="197"/>
-      <c r="I36" s="197"/>
-      <c r="J36" s="197"/>
-      <c r="K36" s="197"/>
-      <c r="L36" s="197"/>
-      <c r="M36" s="197"/>
-      <c r="N36" s="197"/>
-      <c r="O36" s="197"/>
-      <c r="P36" s="197"/>
-      <c r="Q36" s="197"/>
-      <c r="R36" s="197"/>
-      <c r="S36" s="197"/>
-      <c r="T36" s="197"/>
-      <c r="U36" s="197"/>
-      <c r="V36" s="234"/>
+      <c r="B36" s="168"/>
+      <c r="C36" s="168"/>
+      <c r="D36" s="168"/>
+      <c r="E36" s="168"/>
+      <c r="F36" s="168"/>
+      <c r="G36" s="168"/>
+      <c r="H36" s="168"/>
+      <c r="I36" s="168"/>
+      <c r="J36" s="168"/>
+      <c r="K36" s="168"/>
+      <c r="L36" s="168"/>
+      <c r="M36" s="168"/>
+      <c r="N36" s="168"/>
+      <c r="O36" s="168"/>
+      <c r="P36" s="168"/>
+      <c r="Q36" s="168"/>
+      <c r="R36" s="168"/>
+      <c r="S36" s="168"/>
+      <c r="T36" s="168"/>
+      <c r="U36" s="168"/>
+      <c r="V36" s="207"/>
       <c r="W36" s="10"/>
       <c r="X36" s="10"/>
       <c r="Y36" s="10"/>
@@ -34465,14 +34468,14 @@
       <c r="AD36" s="10"/>
     </row>
     <row r="37" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="235" t="s">
+      <c r="A37" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="253" t="s">
+      <c r="B37" s="216" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="241"/>
-      <c r="D37" s="254" t="s">
+      <c r="C37" s="217"/>
+      <c r="D37" s="159" t="s">
         <v>82</v>
       </c>
       <c r="E37" s="103">
@@ -34494,7 +34497,7 @@
       <c r="O37" s="102"/>
       <c r="P37" s="102"/>
       <c r="Q37" s="102"/>
-      <c r="R37" s="102"/>
+      <c r="R37" s="127"/>
       <c r="S37" s="104"/>
       <c r="T37" s="102"/>
       <c r="U37" s="102"/>
@@ -34509,13 +34512,13 @@
       <c r="AD37" s="10"/>
     </row>
     <row r="38" spans="1:30" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="236"/>
-      <c r="B38" s="240" t="s">
-        <v>19</v>
+      <c r="A38" s="209"/>
+      <c r="B38" s="218" t="s">
+        <v>83</v>
       </c>
-      <c r="C38" s="241"/>
+      <c r="C38" s="217"/>
       <c r="D38" s="102" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E38" s="103">
         <v>43935</v>
@@ -34551,8 +34554,8 @@
       <c r="AD38" s="59"/>
     </row>
     <row r="39" spans="1:30" s="56" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="236"/>
-      <c r="B39" s="204" t="s">
+      <c r="A39" s="209"/>
+      <c r="B39" s="252" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="105" t="s">
@@ -34595,8 +34598,8 @@
       <c r="AD39" s="59"/>
     </row>
     <row r="40" spans="1:30" s="56" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="236"/>
-      <c r="B40" s="205"/>
+      <c r="A40" s="209"/>
+      <c r="B40" s="253"/>
       <c r="C40" s="105" t="s">
         <v>22</v>
       </c>
@@ -34637,8 +34640,8 @@
       <c r="AD40" s="59"/>
     </row>
     <row r="41" spans="1:30" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="236"/>
-      <c r="B41" s="206"/>
+      <c r="A41" s="209"/>
+      <c r="B41" s="254"/>
       <c r="C41" s="105" t="s">
         <v>61</v>
       </c>
@@ -34679,8 +34682,8 @@
       <c r="AD41" s="59"/>
     </row>
     <row r="42" spans="1:30" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="236"/>
-      <c r="B42" s="204" t="s">
+      <c r="A42" s="209"/>
+      <c r="B42" s="252" t="s">
         <v>60</v>
       </c>
       <c r="C42" s="105" t="s">
@@ -34723,8 +34726,8 @@
       <c r="AD42" s="59"/>
     </row>
     <row r="43" spans="1:30" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="236"/>
-      <c r="B43" s="205"/>
+      <c r="A43" s="209"/>
+      <c r="B43" s="253"/>
       <c r="C43" s="105" t="s">
         <v>22</v>
       </c>
@@ -34765,8 +34768,8 @@
       <c r="AD43" s="59"/>
     </row>
     <row r="44" spans="1:30" s="56" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="236"/>
-      <c r="B44" s="206"/>
+      <c r="A44" s="209"/>
+      <c r="B44" s="254"/>
       <c r="C44" s="105" t="s">
         <v>61</v>
       </c>
@@ -34807,30 +34810,30 @@
       <c r="AD44" s="59"/>
     </row>
     <row r="45" spans="1:30" s="56" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="190" t="s">
+      <c r="A45" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="190"/>
-      <c r="C45" s="190"/>
-      <c r="D45" s="190"/>
-      <c r="E45" s="190"/>
-      <c r="F45" s="190"/>
-      <c r="G45" s="190"/>
-      <c r="H45" s="190"/>
-      <c r="I45" s="190"/>
-      <c r="J45" s="190"/>
-      <c r="K45" s="190"/>
-      <c r="L45" s="190"/>
-      <c r="M45" s="190"/>
-      <c r="N45" s="190"/>
-      <c r="O45" s="190"/>
-      <c r="P45" s="190"/>
-      <c r="Q45" s="190"/>
-      <c r="R45" s="190"/>
-      <c r="S45" s="190"/>
-      <c r="T45" s="190"/>
-      <c r="U45" s="190"/>
-      <c r="V45" s="191"/>
+      <c r="B45" s="160"/>
+      <c r="C45" s="160"/>
+      <c r="D45" s="160"/>
+      <c r="E45" s="160"/>
+      <c r="F45" s="160"/>
+      <c r="G45" s="160"/>
+      <c r="H45" s="160"/>
+      <c r="I45" s="160"/>
+      <c r="J45" s="160"/>
+      <c r="K45" s="160"/>
+      <c r="L45" s="160"/>
+      <c r="M45" s="160"/>
+      <c r="N45" s="160"/>
+      <c r="O45" s="160"/>
+      <c r="P45" s="160"/>
+      <c r="Q45" s="160"/>
+      <c r="R45" s="160"/>
+      <c r="S45" s="160"/>
+      <c r="T45" s="160"/>
+      <c r="U45" s="160"/>
+      <c r="V45" s="161"/>
       <c r="W45" s="10"/>
       <c r="X45" s="10"/>
       <c r="Y45" s="10"/>
@@ -34844,10 +34847,10 @@
       <c r="A46" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="202" t="s">
+      <c r="B46" s="250" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="203"/>
+      <c r="C46" s="251"/>
       <c r="D46" s="114" t="s">
         <v>20</v>
       </c>
@@ -65574,19 +65577,19 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A36:V36"/>
-    <mergeCell ref="A37:A44"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A45:V45"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A12:A22"/>
@@ -65603,19 +65606,19 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A45:V45"/>
+    <mergeCell ref="A36:V36"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D34:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>